<commit_message>
added Breusch Pagan Test
</commit_message>
<xml_diff>
--- a/OLS_Results_Bottom.xlsx
+++ b/OLS_Results_Bottom.xlsx
@@ -22,10 +22,10 @@
     <t>std err</t>
   </si>
   <si>
-    <t>t</t>
+    <t>z</t>
   </si>
   <si>
-    <t>P&gt;|t|</t>
+    <t>P&gt;|z|</t>
   </si>
   <si>
     <t>[0.025</t>
@@ -501,19 +501,19 @@
         <v>0.6146</v>
       </c>
       <c r="C2">
-        <v>0.405</v>
+        <v>0.434</v>
       </c>
       <c r="D2">
-        <v>1.519</v>
+        <v>1.417</v>
       </c>
       <c r="E2">
-        <v>0.132</v>
+        <v>0.157</v>
       </c>
       <c r="F2">
-        <v>-0.187</v>
+        <v>-0.236</v>
       </c>
       <c r="G2">
-        <v>1.417</v>
+        <v>1.465</v>
       </c>
       <c r="H2" t="s">
         <v>20</v>
@@ -527,19 +527,19 @@
         <v>0.0508</v>
       </c>
       <c r="C3">
-        <v>0.036</v>
+        <v>0.029</v>
       </c>
       <c r="D3">
-        <v>1.425</v>
+        <v>1.748</v>
       </c>
       <c r="E3">
-        <v>0.157</v>
+        <v>0.08</v>
       </c>
       <c r="F3">
-        <v>-0.02</v>
+        <v>-0.006</v>
       </c>
       <c r="G3">
-        <v>0.121</v>
+        <v>0.108</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
@@ -553,19 +553,19 @@
         <v>-0.2492</v>
       </c>
       <c r="C4">
-        <v>0.067</v>
+        <v>0.09</v>
       </c>
       <c r="D4">
-        <v>-3.716</v>
+        <v>-2.77</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.006</v>
       </c>
       <c r="F4">
-        <v>-0.382</v>
+        <v>-0.426</v>
       </c>
       <c r="G4">
-        <v>-0.116</v>
+        <v>-0.073</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -582,7 +582,7 @@
         <v>0.004</v>
       </c>
       <c r="D5">
-        <v>3.578</v>
+        <v>3.365</v>
       </c>
       <c r="E5">
         <v>0.001</v>
@@ -591,7 +591,7 @@
         <v>0.006</v>
       </c>
       <c r="G5">
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -605,19 +605,19 @@
         <v>-0.0584</v>
       </c>
       <c r="C6">
-        <v>0.016</v>
+        <v>0.022</v>
       </c>
       <c r="D6">
-        <v>-3.71</v>
+        <v>-2.702</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="F6">
-        <v>-0.09</v>
+        <v>-0.101</v>
       </c>
       <c r="G6">
-        <v>-0.027</v>
+        <v>-0.016</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -631,19 +631,19 @@
         <v>0.0003</v>
       </c>
       <c r="C7">
-        <v>0.006999999999999999</v>
+        <v>0.006</v>
       </c>
       <c r="D7">
-        <v>0.045</v>
+        <v>0.049</v>
       </c>
       <c r="E7">
-        <v>0.965</v>
+        <v>0.961</v>
       </c>
       <c r="F7">
-        <v>-0.014</v>
+        <v>-0.012</v>
       </c>
       <c r="G7">
-        <v>0.015</v>
+        <v>0.013</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -657,19 +657,19 @@
         <v>-0.0307</v>
       </c>
       <c r="C8">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="D8">
-        <v>-2.087</v>
+        <v>-2.181</v>
       </c>
       <c r="E8">
-        <v>0.039</v>
+        <v>0.029</v>
       </c>
       <c r="F8">
-        <v>-0.06</v>
+        <v>-0.058</v>
       </c>
       <c r="G8">
-        <v>-0.002</v>
+        <v>-0.003</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -683,19 +683,19 @@
         <v>0.009599999999999999</v>
       </c>
       <c r="C9">
-        <v>0.008</v>
+        <v>0.014</v>
       </c>
       <c r="D9">
-        <v>1.133</v>
+        <v>0.679</v>
       </c>
       <c r="E9">
-        <v>0.26</v>
+        <v>0.4970000000000001</v>
       </c>
       <c r="F9">
-        <v>-0.006999999999999999</v>
+        <v>-0.018</v>
       </c>
       <c r="G9">
-        <v>0.026</v>
+        <v>0.03700000000000001</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
@@ -712,16 +712,16 @@
         <v>0.004</v>
       </c>
       <c r="D10">
-        <v>-0.763</v>
+        <v>-0.892</v>
       </c>
       <c r="E10">
-        <v>0.447</v>
+        <v>0.3720000000000001</v>
       </c>
       <c r="F10">
-        <v>-0.012</v>
+        <v>-0.011</v>
       </c>
       <c r="G10">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
@@ -735,19 +735,19 @@
         <v>0.1357</v>
       </c>
       <c r="C11">
-        <v>0.038</v>
+        <v>0.048</v>
       </c>
       <c r="D11">
-        <v>3.572</v>
+        <v>2.825</v>
       </c>
       <c r="E11">
-        <v>0.001</v>
+        <v>0.005</v>
       </c>
       <c r="F11">
-        <v>0.06</v>
+        <v>0.042</v>
       </c>
       <c r="G11">
-        <v>0.211</v>
+        <v>0.23</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -761,19 +761,19 @@
         <v>0.245</v>
       </c>
       <c r="C12">
-        <v>0.049</v>
+        <v>0.067</v>
       </c>
       <c r="D12">
-        <v>4.968</v>
+        <v>3.684</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0.147</v>
+        <v>0.115</v>
       </c>
       <c r="G12">
-        <v>0.343</v>
+        <v>0.375</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -787,19 +787,19 @@
         <v>-0.0278</v>
       </c>
       <c r="C13">
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
       <c r="D13">
-        <v>-5.149</v>
+        <v>-4.403</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>-0.038</v>
+        <v>-0.04</v>
       </c>
       <c r="G13">
-        <v>-0.017</v>
+        <v>-0.015</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -813,19 +813,19 @@
         <v>0.0312</v>
       </c>
       <c r="C14">
+        <v>0.011</v>
+      </c>
+      <c r="D14">
+        <v>2.817</v>
+      </c>
+      <c r="E14">
+        <v>0.005</v>
+      </c>
+      <c r="F14">
         <v>0.009000000000000001</v>
       </c>
-      <c r="D14">
-        <v>3.566</v>
-      </c>
-      <c r="E14">
-        <v>0.001</v>
-      </c>
-      <c r="F14">
-        <v>0.014</v>
-      </c>
       <c r="G14">
-        <v>0.049</v>
+        <v>0.053</v>
       </c>
       <c r="H14" t="s">
         <v>20</v>
@@ -839,19 +839,19 @@
         <v>0.3306</v>
       </c>
       <c r="C15">
-        <v>0.31</v>
+        <v>0.24</v>
       </c>
       <c r="D15">
-        <v>1.066</v>
+        <v>1.379</v>
       </c>
       <c r="E15">
-        <v>0.289</v>
+        <v>0.168</v>
       </c>
       <c r="F15">
-        <v>-0.284</v>
+        <v>-0.139</v>
       </c>
       <c r="G15">
-        <v>0.945</v>
+        <v>0.8</v>
       </c>
       <c r="H15" t="s">
         <v>21</v>
@@ -865,19 +865,19 @@
         <v>-0.015</v>
       </c>
       <c r="C16">
-        <v>0.027</v>
+        <v>0.025</v>
       </c>
       <c r="D16">
-        <v>-0.55</v>
+        <v>-0.609</v>
       </c>
       <c r="E16">
-        <v>0.583</v>
+        <v>0.5429999999999999</v>
       </c>
       <c r="F16">
-        <v>-0.06900000000000001</v>
+        <v>-0.063</v>
       </c>
       <c r="G16">
-        <v>0.039</v>
+        <v>0.033</v>
       </c>
       <c r="H16" t="s">
         <v>21</v>
@@ -891,19 +891,19 @@
         <v>-0.0883</v>
       </c>
       <c r="C17">
-        <v>0.051</v>
+        <v>0.04099999999999999</v>
       </c>
       <c r="D17">
-        <v>-1.719</v>
+        <v>-2.174</v>
       </c>
       <c r="E17">
-        <v>0.08800000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="F17">
-        <v>-0.19</v>
+        <v>-0.168</v>
       </c>
       <c r="G17">
-        <v>0.014</v>
+        <v>-0.009000000000000001</v>
       </c>
       <c r="H17" t="s">
         <v>21</v>
@@ -920,10 +920,10 @@
         <v>0.003</v>
       </c>
       <c r="D18">
-        <v>0.44</v>
+        <v>0.446</v>
       </c>
       <c r="E18">
-        <v>0.6609999999999999</v>
+        <v>0.6559999999999999</v>
       </c>
       <c r="F18">
         <v>-0.005</v>
@@ -946,7 +946,7 @@
         <v>0.012</v>
       </c>
       <c r="D19">
-        <v>-3.016</v>
+        <v>-3.012</v>
       </c>
       <c r="E19">
         <v>0.003</v>
@@ -955,7 +955,7 @@
         <v>-0.06</v>
       </c>
       <c r="G19">
-        <v>-0.012</v>
+        <v>-0.013</v>
       </c>
       <c r="H19" t="s">
         <v>21</v>
@@ -969,19 +969,19 @@
         <v>-0.0012</v>
       </c>
       <c r="C20">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="D20">
-        <v>-0.21</v>
+        <v>-0.605</v>
       </c>
       <c r="E20">
-        <v>0.8340000000000001</v>
+        <v>0.545</v>
       </c>
       <c r="F20">
-        <v>-0.012</v>
+        <v>-0.005</v>
       </c>
       <c r="G20">
-        <v>0.01</v>
+        <v>0.003</v>
       </c>
       <c r="H20" t="s">
         <v>21</v>
@@ -995,19 +995,19 @@
         <v>-0.0055</v>
       </c>
       <c r="C21">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="D21">
-        <v>-0.492</v>
+        <v>-0.5720000000000001</v>
       </c>
       <c r="E21">
-        <v>0.624</v>
+        <v>0.5670000000000001</v>
       </c>
       <c r="F21">
-        <v>-0.028</v>
+        <v>-0.025</v>
       </c>
       <c r="G21">
-        <v>0.017</v>
+        <v>0.013</v>
       </c>
       <c r="H21" t="s">
         <v>21</v>
@@ -1021,19 +1021,19 @@
         <v>0.001</v>
       </c>
       <c r="C22">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="D22">
-        <v>0.147</v>
+        <v>0.175</v>
       </c>
       <c r="E22">
-        <v>0.884</v>
+        <v>0.861</v>
       </c>
       <c r="F22">
-        <v>-0.012</v>
+        <v>-0.01</v>
       </c>
       <c r="G22">
-        <v>0.014</v>
+        <v>0.012</v>
       </c>
       <c r="H22" t="s">
         <v>21</v>
@@ -1050,16 +1050,16 @@
         <v>0.003</v>
       </c>
       <c r="D23">
-        <v>-1.434</v>
+        <v>-1.605</v>
       </c>
       <c r="E23">
-        <v>0.155</v>
+        <v>0.108</v>
       </c>
       <c r="F23">
-        <v>-0.012</v>
+        <v>-0.011</v>
       </c>
       <c r="G23">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="H23" t="s">
         <v>21</v>
@@ -1073,19 +1073,19 @@
         <v>0.0471</v>
       </c>
       <c r="C24">
-        <v>0.029</v>
+        <v>0.027</v>
       </c>
       <c r="D24">
-        <v>1.617</v>
+        <v>1.751</v>
       </c>
       <c r="E24">
-        <v>0.109</v>
+        <v>0.08</v>
       </c>
       <c r="F24">
-        <v>-0.011</v>
+        <v>-0.006</v>
       </c>
       <c r="G24">
-        <v>0.105</v>
+        <v>0.1</v>
       </c>
       <c r="H24" t="s">
         <v>21</v>
@@ -1099,19 +1099,19 @@
         <v>0.0592</v>
       </c>
       <c r="C25">
-        <v>0.038</v>
+        <v>0.023</v>
       </c>
       <c r="D25">
-        <v>1.565</v>
+        <v>2.539</v>
       </c>
       <c r="E25">
-        <v>0.12</v>
+        <v>0.011</v>
       </c>
       <c r="F25">
-        <v>-0.016</v>
+        <v>0.013</v>
       </c>
       <c r="G25">
-        <v>0.134</v>
+        <v>0.105</v>
       </c>
       <c r="H25" t="s">
         <v>21</v>
@@ -1125,19 +1125,19 @@
         <v>-0.0041</v>
       </c>
       <c r="C26">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="D26">
-        <v>-0.988</v>
+        <v>-1.318</v>
       </c>
       <c r="E26">
-        <v>0.325</v>
+        <v>0.188</v>
       </c>
       <c r="F26">
-        <v>-0.012</v>
+        <v>-0.01</v>
       </c>
       <c r="G26">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="H26" t="s">
         <v>21</v>
@@ -1151,19 +1151,19 @@
         <v>-0.0032</v>
       </c>
       <c r="C27">
-        <v>0.006999999999999999</v>
+        <v>0.005</v>
       </c>
       <c r="D27">
-        <v>-0.473</v>
+        <v>-0.643</v>
       </c>
       <c r="E27">
-        <v>0.637</v>
+        <v>0.52</v>
       </c>
       <c r="F27">
-        <v>-0.016</v>
+        <v>-0.013</v>
       </c>
       <c r="G27">
-        <v>0.01</v>
+        <v>0.006</v>
       </c>
       <c r="H27" t="s">
         <v>21</v>
@@ -1177,19 +1177,19 @@
         <v>-3.8117</v>
       </c>
       <c r="C28">
-        <v>2.01</v>
+        <v>3.484</v>
       </c>
       <c r="D28">
-        <v>-1.896</v>
+        <v>-1.094</v>
       </c>
       <c r="E28">
-        <v>0.061</v>
+        <v>0.274</v>
       </c>
       <c r="F28">
-        <v>-7.796</v>
+        <v>-10.64</v>
       </c>
       <c r="G28">
-        <v>0.173</v>
+        <v>3.017</v>
       </c>
       <c r="H28" t="s">
         <v>22</v>
@@ -1203,19 +1203,19 @@
         <v>-0.0324</v>
       </c>
       <c r="C29">
-        <v>0.177</v>
+        <v>0.131</v>
       </c>
       <c r="D29">
-        <v>-0.183</v>
+        <v>-0.247</v>
       </c>
       <c r="E29">
-        <v>0.855</v>
+        <v>0.805</v>
       </c>
       <c r="F29">
-        <v>-0.383</v>
+        <v>-0.29</v>
       </c>
       <c r="G29">
-        <v>0.319</v>
+        <v>0.225</v>
       </c>
       <c r="H29" t="s">
         <v>22</v>
@@ -1229,19 +1229,19 @@
         <v>-0.2388</v>
       </c>
       <c r="C30">
-        <v>0.333</v>
+        <v>0.268</v>
       </c>
       <c r="D30">
-        <v>-0.7170000000000001</v>
+        <v>-0.889</v>
       </c>
       <c r="E30">
-        <v>0.475</v>
+        <v>0.374</v>
       </c>
       <c r="F30">
-        <v>-0.899</v>
+        <v>-0.765</v>
       </c>
       <c r="G30">
-        <v>0.422</v>
+        <v>0.287</v>
       </c>
       <c r="H30" t="s">
         <v>22</v>
@@ -1255,19 +1255,19 @@
         <v>-0.0001</v>
       </c>
       <c r="C31">
-        <v>0.02</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="D31">
-        <v>-0.006</v>
+        <v>-0.014</v>
       </c>
       <c r="E31">
-        <v>0.995</v>
+        <v>0.9890000000000001</v>
       </c>
       <c r="F31">
-        <v>-0.039</v>
+        <v>-0.019</v>
       </c>
       <c r="G31">
-        <v>0.039</v>
+        <v>0.018</v>
       </c>
       <c r="H31" t="s">
         <v>22</v>
@@ -1281,19 +1281,19 @@
         <v>0.193</v>
       </c>
       <c r="C32">
-        <v>0.078</v>
+        <v>0.16</v>
       </c>
       <c r="D32">
-        <v>2.466</v>
+        <v>1.206</v>
       </c>
       <c r="E32">
-        <v>0.015</v>
+        <v>0.228</v>
       </c>
       <c r="F32">
-        <v>0.038</v>
+        <v>-0.121</v>
       </c>
       <c r="G32">
-        <v>0.348</v>
+        <v>0.507</v>
       </c>
       <c r="H32" t="s">
         <v>22</v>
@@ -1307,19 +1307,19 @@
         <v>-0.0004</v>
       </c>
       <c r="C33">
-        <v>0.036</v>
+        <v>0.027</v>
       </c>
       <c r="D33">
-        <v>-0.013</v>
+        <v>-0.017</v>
       </c>
       <c r="E33">
-        <v>0.99</v>
+        <v>0.987</v>
       </c>
       <c r="F33">
-        <v>-0.07099999999999999</v>
+        <v>-0.053</v>
       </c>
       <c r="G33">
-        <v>0.07000000000000001</v>
+        <v>0.052</v>
       </c>
       <c r="H33" t="s">
         <v>22</v>
@@ -1333,19 +1333,19 @@
         <v>0.1369</v>
       </c>
       <c r="C34">
-        <v>0.073</v>
+        <v>0.113</v>
       </c>
       <c r="D34">
-        <v>1.873</v>
+        <v>1.207</v>
       </c>
       <c r="E34">
-        <v>0.064</v>
+        <v>0.227</v>
       </c>
       <c r="F34">
-        <v>-0.008</v>
+        <v>-0.08500000000000001</v>
       </c>
       <c r="G34">
-        <v>0.282</v>
+        <v>0.359</v>
       </c>
       <c r="H34" t="s">
         <v>22</v>
@@ -1359,19 +1359,19 @@
         <v>-0.0218</v>
       </c>
       <c r="C35">
-        <v>0.042</v>
+        <v>0.025</v>
       </c>
       <c r="D35">
-        <v>-0.517</v>
+        <v>-0.871</v>
       </c>
       <c r="E35">
-        <v>0.606</v>
+        <v>0.384</v>
       </c>
       <c r="F35">
-        <v>-0.105</v>
+        <v>-0.07099999999999999</v>
       </c>
       <c r="G35">
-        <v>0.062</v>
+        <v>0.027</v>
       </c>
       <c r="H35" t="s">
         <v>22</v>
@@ -1385,19 +1385,19 @@
         <v>0.0201</v>
       </c>
       <c r="C36">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
       <c r="D36">
-        <v>0.9009999999999999</v>
+        <v>1.011</v>
       </c>
       <c r="E36">
-        <v>0.37</v>
+        <v>0.312</v>
       </c>
       <c r="F36">
-        <v>-0.024</v>
+        <v>-0.019</v>
       </c>
       <c r="G36">
-        <v>0.064</v>
+        <v>0.059</v>
       </c>
       <c r="H36" t="s">
         <v>22</v>
@@ -1411,19 +1411,19 @@
         <v>0.5164</v>
       </c>
       <c r="C37">
-        <v>0.189</v>
+        <v>0.402</v>
       </c>
       <c r="D37">
-        <v>2.736</v>
+        <v>1.285</v>
       </c>
       <c r="E37">
-        <v>0.006999999999999999</v>
+        <v>0.199</v>
       </c>
       <c r="F37">
-        <v>0.142</v>
+        <v>-0.271</v>
       </c>
       <c r="G37">
-        <v>0.8909999999999999</v>
+        <v>1.304</v>
       </c>
       <c r="H37" t="s">
         <v>22</v>
@@ -1437,19 +1437,19 @@
         <v>-0.0901</v>
       </c>
       <c r="C38">
-        <v>0.245</v>
+        <v>0.112</v>
       </c>
       <c r="D38">
-        <v>-0.368</v>
+        <v>-0.804</v>
       </c>
       <c r="E38">
-        <v>0.7140000000000001</v>
+        <v>0.421</v>
       </c>
       <c r="F38">
-        <v>-0.5760000000000001</v>
+        <v>-0.31</v>
       </c>
       <c r="G38">
-        <v>0.396</v>
+        <v>0.13</v>
       </c>
       <c r="H38" t="s">
         <v>22</v>
@@ -1466,10 +1466,10 @@
         <v>0.027</v>
       </c>
       <c r="D39">
-        <v>1.017</v>
+        <v>1.009</v>
       </c>
       <c r="E39">
-        <v>0.312</v>
+        <v>0.313</v>
       </c>
       <c r="F39">
         <v>-0.026</v>
@@ -1489,19 +1489,19 @@
         <v>-0.0094</v>
       </c>
       <c r="C40">
-        <v>0.043</v>
+        <v>0.017</v>
       </c>
       <c r="D40">
-        <v>-0.217</v>
+        <v>-0.544</v>
       </c>
       <c r="E40">
-        <v>0.8290000000000001</v>
+        <v>0.586</v>
       </c>
       <c r="F40">
-        <v>-0.096</v>
+        <v>-0.043</v>
       </c>
       <c r="G40">
-        <v>0.077</v>
+        <v>0.025</v>
       </c>
       <c r="H40" t="s">
         <v>22</v>
@@ -1515,19 +1515,19 @@
         <v>0.9184</v>
       </c>
       <c r="C41">
-        <v>0.555</v>
+        <v>0.865</v>
       </c>
       <c r="D41">
-        <v>1.656</v>
+        <v>1.062</v>
       </c>
       <c r="E41">
-        <v>0.101</v>
+        <v>0.288</v>
       </c>
       <c r="F41">
-        <v>-0.181</v>
+        <v>-0.777</v>
       </c>
       <c r="G41">
-        <v>2.018</v>
+        <v>2.614</v>
       </c>
       <c r="H41" t="s">
         <v>23</v>
@@ -1541,19 +1541,19 @@
         <v>0.0154</v>
       </c>
       <c r="C42">
-        <v>0.049</v>
+        <v>0.033</v>
       </c>
       <c r="D42">
-        <v>0.315</v>
+        <v>0.461</v>
       </c>
       <c r="E42">
-        <v>0.753</v>
+        <v>0.645</v>
       </c>
       <c r="F42">
-        <v>-0.081</v>
+        <v>-0.05</v>
       </c>
       <c r="G42">
-        <v>0.112</v>
+        <v>0.081</v>
       </c>
       <c r="H42" t="s">
         <v>23</v>
@@ -1567,19 +1567,19 @@
         <v>0.0215</v>
       </c>
       <c r="C43">
-        <v>0.092</v>
+        <v>0.073</v>
       </c>
       <c r="D43">
-        <v>0.234</v>
+        <v>0.297</v>
       </c>
       <c r="E43">
-        <v>0.8149999999999999</v>
+        <v>0.7659999999999999</v>
       </c>
       <c r="F43">
-        <v>-0.161</v>
+        <v>-0.121</v>
       </c>
       <c r="G43">
-        <v>0.204</v>
+        <v>0.164</v>
       </c>
       <c r="H43" t="s">
         <v>23</v>
@@ -1593,19 +1593,19 @@
         <v>0.0023</v>
       </c>
       <c r="C44">
-        <v>0.005</v>
+        <v>0.003</v>
       </c>
       <c r="D44">
-        <v>0.429</v>
+        <v>0.802</v>
       </c>
       <c r="E44">
-        <v>0.669</v>
+        <v>0.422</v>
       </c>
       <c r="F44">
-        <v>-0.009000000000000001</v>
+        <v>-0.003</v>
       </c>
       <c r="G44">
-        <v>0.013</v>
+        <v>0.008</v>
       </c>
       <c r="H44" t="s">
         <v>23</v>
@@ -1619,19 +1619,19 @@
         <v>-0.0555</v>
       </c>
       <c r="C45">
-        <v>0.022</v>
+        <v>0.04099999999999999</v>
       </c>
       <c r="D45">
-        <v>-2.568</v>
+        <v>-1.344</v>
       </c>
       <c r="E45">
-        <v>0.012</v>
+        <v>0.179</v>
       </c>
       <c r="F45">
-        <v>-0.098</v>
+        <v>-0.136</v>
       </c>
       <c r="G45">
-        <v>-0.013</v>
+        <v>0.025</v>
       </c>
       <c r="H45" t="s">
         <v>23</v>
@@ -1645,19 +1645,19 @@
         <v>0.0023</v>
       </c>
       <c r="C46">
-        <v>0.01</v>
+        <v>0.006</v>
       </c>
       <c r="D46">
-        <v>0.23</v>
+        <v>0.402</v>
       </c>
       <c r="E46">
-        <v>0.8179999999999999</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="F46">
-        <v>-0.017</v>
+        <v>-0.009000000000000001</v>
       </c>
       <c r="G46">
-        <v>0.022</v>
+        <v>0.013</v>
       </c>
       <c r="H46" t="s">
         <v>23</v>
@@ -1671,19 +1671,19 @@
         <v>-0.0373</v>
       </c>
       <c r="C47">
+        <v>0.029</v>
+      </c>
+      <c r="D47">
+        <v>-1.266</v>
+      </c>
+      <c r="E47">
+        <v>0.206</v>
+      </c>
+      <c r="F47">
+        <v>-0.095</v>
+      </c>
+      <c r="G47">
         <v>0.02</v>
-      </c>
-      <c r="D47">
-        <v>-1.849</v>
-      </c>
-      <c r="E47">
-        <v>0.067</v>
-      </c>
-      <c r="F47">
-        <v>-0.077</v>
-      </c>
-      <c r="G47">
-        <v>0.003</v>
       </c>
       <c r="H47" t="s">
         <v>23</v>
@@ -1697,19 +1697,19 @@
         <v>0.0089</v>
       </c>
       <c r="C48">
-        <v>0.012</v>
+        <v>0.008</v>
       </c>
       <c r="D48">
-        <v>0.762</v>
+        <v>1.132</v>
       </c>
       <c r="E48">
-        <v>0.447</v>
+        <v>0.258</v>
       </c>
       <c r="F48">
-        <v>-0.014</v>
+        <v>-0.006</v>
       </c>
       <c r="G48">
-        <v>0.032</v>
+        <v>0.024</v>
       </c>
       <c r="H48" t="s">
         <v>23</v>
@@ -1726,16 +1726,16 @@
         <v>0.006</v>
       </c>
       <c r="D49">
-        <v>-0.95</v>
+        <v>-1.057</v>
       </c>
       <c r="E49">
-        <v>0.344</v>
+        <v>0.291</v>
       </c>
       <c r="F49">
-        <v>-0.018</v>
+        <v>-0.017</v>
       </c>
       <c r="G49">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="H49" t="s">
         <v>23</v>
@@ -1749,19 +1749,19 @@
         <v>-0.1149</v>
       </c>
       <c r="C50">
-        <v>0.052</v>
+        <v>0.102</v>
       </c>
       <c r="D50">
-        <v>-2.206</v>
+        <v>-1.129</v>
       </c>
       <c r="E50">
-        <v>0.029</v>
+        <v>0.259</v>
       </c>
       <c r="F50">
-        <v>-0.218</v>
+        <v>-0.314</v>
       </c>
       <c r="G50">
-        <v>-0.012</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="H50" t="s">
         <v>23</v>
@@ -1775,19 +1775,19 @@
         <v>0.07439999999999999</v>
       </c>
       <c r="C51">
-        <v>0.068</v>
+        <v>0.04</v>
       </c>
       <c r="D51">
-        <v>1.101</v>
+        <v>1.881</v>
       </c>
       <c r="E51">
-        <v>0.273</v>
+        <v>0.06</v>
       </c>
       <c r="F51">
-        <v>-0.06</v>
+        <v>-0.003</v>
       </c>
       <c r="G51">
-        <v>0.208</v>
+        <v>0.152</v>
       </c>
       <c r="H51" t="s">
         <v>23</v>
@@ -1804,10 +1804,10 @@
         <v>0.006999999999999999</v>
       </c>
       <c r="D52">
-        <v>-1.419</v>
+        <v>-1.432</v>
       </c>
       <c r="E52">
-        <v>0.159</v>
+        <v>0.152</v>
       </c>
       <c r="F52">
         <v>-0.025</v>
@@ -1827,19 +1827,19 @@
         <v>0.0062</v>
       </c>
       <c r="C53">
-        <v>0.012</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="D53">
-        <v>0.52</v>
+        <v>0.915</v>
       </c>
       <c r="E53">
-        <v>0.604</v>
+        <v>0.36</v>
       </c>
       <c r="F53">
-        <v>-0.018</v>
+        <v>-0.006999999999999999</v>
       </c>
       <c r="G53">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="H53" t="s">
         <v>23</v>
@@ -1853,19 +1853,19 @@
         <v>-0.2598</v>
       </c>
       <c r="C54">
-        <v>0.604</v>
+        <v>0.467</v>
       </c>
       <c r="D54">
-        <v>-0.43</v>
+        <v>-0.556</v>
       </c>
       <c r="E54">
-        <v>0.6679999999999999</v>
+        <v>0.578</v>
       </c>
       <c r="F54">
-        <v>-1.457</v>
+        <v>-1.176</v>
       </c>
       <c r="G54">
-        <v>0.9379999999999999</v>
+        <v>0.6559999999999999</v>
       </c>
       <c r="H54" t="s">
         <v>24</v>
@@ -1879,19 +1879,19 @@
         <v>-0.0722</v>
       </c>
       <c r="C55">
-        <v>0.053</v>
+        <v>0.049</v>
       </c>
       <c r="D55">
-        <v>-1.357</v>
+        <v>-1.463</v>
       </c>
       <c r="E55">
-        <v>0.178</v>
+        <v>0.144</v>
       </c>
       <c r="F55">
-        <v>-0.178</v>
+        <v>-0.169</v>
       </c>
       <c r="G55">
-        <v>0.033</v>
+        <v>0.025</v>
       </c>
       <c r="H55" t="s">
         <v>24</v>
@@ -1905,19 +1905,19 @@
         <v>0.1273</v>
       </c>
       <c r="C56">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="D56">
-        <v>1.271</v>
+        <v>1.41</v>
       </c>
       <c r="E56">
-        <v>0.206</v>
+        <v>0.159</v>
       </c>
       <c r="F56">
-        <v>-0.07099999999999999</v>
+        <v>-0.05</v>
       </c>
       <c r="G56">
-        <v>0.326</v>
+        <v>0.304</v>
       </c>
       <c r="H56" t="s">
         <v>24</v>
@@ -1934,10 +1934,10 @@
         <v>0.006</v>
       </c>
       <c r="D57">
-        <v>-0.347</v>
+        <v>-0.336</v>
       </c>
       <c r="E57">
-        <v>0.73</v>
+        <v>0.737</v>
       </c>
       <c r="F57">
         <v>-0.014</v>
@@ -1957,19 +1957,19 @@
         <v>-0.0144</v>
       </c>
       <c r="C58">
-        <v>0.024</v>
+        <v>0.025</v>
       </c>
       <c r="D58">
-        <v>-0.614</v>
+        <v>-0.5770000000000001</v>
       </c>
       <c r="E58">
-        <v>0.54</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="F58">
-        <v>-0.061</v>
+        <v>-0.064</v>
       </c>
       <c r="G58">
-        <v>0.032</v>
+        <v>0.035</v>
       </c>
       <c r="H58" t="s">
         <v>24</v>
@@ -1983,19 +1983,19 @@
         <v>0.0025</v>
       </c>
       <c r="C59">
-        <v>0.011</v>
+        <v>0.006</v>
       </c>
       <c r="D59">
-        <v>0.231</v>
+        <v>0.398</v>
       </c>
       <c r="E59">
-        <v>0.8179999999999999</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="F59">
-        <v>-0.019</v>
+        <v>-0.01</v>
       </c>
       <c r="G59">
-        <v>0.024</v>
+        <v>0.015</v>
       </c>
       <c r="H59" t="s">
         <v>24</v>
@@ -2009,19 +2009,19 @@
         <v>-0.0244</v>
       </c>
       <c r="C60">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
       <c r="D60">
-        <v>-1.111</v>
+        <v>-1.192</v>
       </c>
       <c r="E60">
-        <v>0.269</v>
+        <v>0.233</v>
       </c>
       <c r="F60">
-        <v>-0.068</v>
+        <v>-0.065</v>
       </c>
       <c r="G60">
-        <v>0.019</v>
+        <v>0.016</v>
       </c>
       <c r="H60" t="s">
         <v>24</v>
@@ -2038,10 +2038,10 @@
         <v>0.013</v>
       </c>
       <c r="D61">
-        <v>-0.08800000000000001</v>
+        <v>-0.08900000000000001</v>
       </c>
       <c r="E61">
-        <v>0.93</v>
+        <v>0.929</v>
       </c>
       <c r="F61">
         <v>-0.026</v>
@@ -2061,19 +2061,19 @@
         <v>-0.0086</v>
       </c>
       <c r="C62">
-        <v>0.006999999999999999</v>
+        <v>0.005</v>
       </c>
       <c r="D62">
-        <v>-1.284</v>
+        <v>-1.641</v>
       </c>
       <c r="E62">
-        <v>0.202</v>
+        <v>0.101</v>
       </c>
       <c r="F62">
-        <v>-0.022</v>
+        <v>-0.019</v>
       </c>
       <c r="G62">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="H62" t="s">
         <v>24</v>
@@ -2087,19 +2087,19 @@
         <v>-0.1417</v>
       </c>
       <c r="C63">
-        <v>0.057</v>
+        <v>0.05400000000000001</v>
       </c>
       <c r="D63">
-        <v>-2.497</v>
+        <v>-2.622</v>
       </c>
       <c r="E63">
-        <v>0.014</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="F63">
-        <v>-0.254</v>
+        <v>-0.248</v>
       </c>
       <c r="G63">
-        <v>-0.029</v>
+        <v>-0.036</v>
       </c>
       <c r="H63" t="s">
         <v>24</v>
@@ -2113,19 +2113,19 @@
         <v>0.1702</v>
       </c>
       <c r="C64">
-        <v>0.07400000000000001</v>
+        <v>0.067</v>
       </c>
       <c r="D64">
-        <v>2.311</v>
+        <v>2.547</v>
       </c>
       <c r="E64">
-        <v>0.023</v>
+        <v>0.011</v>
       </c>
       <c r="F64">
-        <v>0.024</v>
+        <v>0.039</v>
       </c>
       <c r="G64">
-        <v>0.316</v>
+        <v>0.301</v>
       </c>
       <c r="H64" t="s">
         <v>24</v>
@@ -2139,19 +2139,19 @@
         <v>0.0121</v>
       </c>
       <c r="C65">
-        <v>0.008</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="D65">
-        <v>1.5</v>
+        <v>1.359</v>
       </c>
       <c r="E65">
-        <v>0.136</v>
+        <v>0.174</v>
       </c>
       <c r="F65">
-        <v>-0.004</v>
+        <v>-0.005</v>
       </c>
       <c r="G65">
-        <v>0.028</v>
+        <v>0.03</v>
       </c>
       <c r="H65" t="s">
         <v>24</v>
@@ -2165,19 +2165,19 @@
         <v>0.0089</v>
       </c>
       <c r="C66">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D66">
-        <v>0.68</v>
+        <v>0.731</v>
       </c>
       <c r="E66">
-        <v>0.498</v>
+        <v>0.465</v>
       </c>
       <c r="F66">
-        <v>-0.017</v>
+        <v>-0.015</v>
       </c>
       <c r="G66">
-        <v>0.035</v>
+        <v>0.033</v>
       </c>
       <c r="H66" t="s">
         <v>24</v>
@@ -2191,19 +2191,19 @@
         <v>2.7757</v>
       </c>
       <c r="C67">
-        <v>1.438</v>
+        <v>2.32</v>
       </c>
       <c r="D67">
-        <v>1.93</v>
+        <v>1.196</v>
       </c>
       <c r="E67">
-        <v>0.05599999999999999</v>
+        <v>0.232</v>
       </c>
       <c r="F67">
-        <v>-0.075</v>
+        <v>-1.772</v>
       </c>
       <c r="G67">
-        <v>5.626</v>
+        <v>7.323</v>
       </c>
       <c r="H67" t="s">
         <v>25</v>
@@ -2217,19 +2217,19 @@
         <v>0.0134</v>
       </c>
       <c r="C68">
-        <v>0.127</v>
+        <v>0.094</v>
       </c>
       <c r="D68">
-        <v>0.106</v>
+        <v>0.143</v>
       </c>
       <c r="E68">
-        <v>0.9159999999999999</v>
+        <v>0.8859999999999999</v>
       </c>
       <c r="F68">
-        <v>-0.238</v>
+        <v>-0.171</v>
       </c>
       <c r="G68">
-        <v>0.265</v>
+        <v>0.198</v>
       </c>
       <c r="H68" t="s">
         <v>25</v>
@@ -2243,19 +2243,19 @@
         <v>0.2162</v>
       </c>
       <c r="C69">
-        <v>0.238</v>
+        <v>0.172</v>
       </c>
       <c r="D69">
-        <v>0.907</v>
+        <v>1.256</v>
       </c>
       <c r="E69">
-        <v>0.366</v>
+        <v>0.209</v>
       </c>
       <c r="F69">
-        <v>-0.256</v>
+        <v>-0.121</v>
       </c>
       <c r="G69">
-        <v>0.6890000000000001</v>
+        <v>0.5539999999999999</v>
       </c>
       <c r="H69" t="s">
         <v>25</v>
@@ -2269,19 +2269,19 @@
         <v>0.0002</v>
       </c>
       <c r="C70">
-        <v>0.014</v>
+        <v>0.006</v>
       </c>
       <c r="D70">
-        <v>0.018</v>
+        <v>0.04099999999999999</v>
       </c>
       <c r="E70">
-        <v>0.986</v>
+        <v>0.968</v>
       </c>
       <c r="F70">
-        <v>-0.028</v>
+        <v>-0.012</v>
       </c>
       <c r="G70">
-        <v>0.028</v>
+        <v>0.012</v>
       </c>
       <c r="H70" t="s">
         <v>25</v>
@@ -2295,19 +2295,19 @@
         <v>-0.1478</v>
       </c>
       <c r="C71">
-        <v>0.05599999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="D71">
-        <v>-2.64</v>
+        <v>-1.35</v>
       </c>
       <c r="E71">
-        <v>0.01</v>
+        <v>0.177</v>
       </c>
       <c r="F71">
-        <v>-0.259</v>
+        <v>-0.362</v>
       </c>
       <c r="G71">
-        <v>-0.03700000000000001</v>
+        <v>0.067</v>
       </c>
       <c r="H71" t="s">
         <v>25</v>
@@ -2321,19 +2321,19 @@
         <v>-0.0004</v>
       </c>
       <c r="C72">
-        <v>0.025</v>
+        <v>0.015</v>
       </c>
       <c r="D72">
-        <v>-0.015</v>
+        <v>-0.025</v>
       </c>
       <c r="E72">
-        <v>0.988</v>
+        <v>0.98</v>
       </c>
       <c r="F72">
-        <v>-0.051</v>
+        <v>-0.031</v>
       </c>
       <c r="G72">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="H72" t="s">
         <v>25</v>
@@ -2347,19 +2347,19 @@
         <v>-0.1002</v>
       </c>
       <c r="C73">
-        <v>0.052</v>
+        <v>0.077</v>
       </c>
       <c r="D73">
-        <v>-1.916</v>
+        <v>-1.305</v>
       </c>
       <c r="E73">
-        <v>0.058</v>
+        <v>0.192</v>
       </c>
       <c r="F73">
-        <v>-0.204</v>
+        <v>-0.251</v>
       </c>
       <c r="G73">
-        <v>0.003</v>
+        <v>0.05</v>
       </c>
       <c r="H73" t="s">
         <v>25</v>
@@ -2373,19 +2373,19 @@
         <v>0.0136</v>
       </c>
       <c r="C74">
-        <v>0.03</v>
+        <v>0.018</v>
       </c>
       <c r="D74">
-        <v>0.453</v>
+        <v>0.742</v>
       </c>
       <c r="E74">
-        <v>0.652</v>
+        <v>0.458</v>
       </c>
       <c r="F74">
-        <v>-0.046</v>
+        <v>-0.022</v>
       </c>
       <c r="G74">
-        <v>0.073</v>
+        <v>0.05</v>
       </c>
       <c r="H74" t="s">
         <v>25</v>
@@ -2399,19 +2399,19 @@
         <v>-0.0207</v>
       </c>
       <c r="C75">
-        <v>0.016</v>
+        <v>0.014</v>
       </c>
       <c r="D75">
-        <v>-1.296</v>
+        <v>-1.477</v>
       </c>
       <c r="E75">
-        <v>0.198</v>
+        <v>0.14</v>
       </c>
       <c r="F75">
-        <v>-0.052</v>
+        <v>-0.048</v>
       </c>
       <c r="G75">
-        <v>0.011</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="H75" t="s">
         <v>25</v>
@@ -2425,19 +2425,19 @@
         <v>-0.3865</v>
       </c>
       <c r="C76">
-        <v>0.135</v>
+        <v>0.272</v>
       </c>
       <c r="D76">
-        <v>-2.861</v>
+        <v>-1.421</v>
       </c>
       <c r="E76">
-        <v>0.005</v>
+        <v>0.155</v>
       </c>
       <c r="F76">
-        <v>-0.654</v>
+        <v>-0.92</v>
       </c>
       <c r="G76">
-        <v>-0.119</v>
+        <v>0.147</v>
       </c>
       <c r="H76" t="s">
         <v>25</v>
@@ -2451,19 +2451,19 @@
         <v>0.1056</v>
       </c>
       <c r="C77">
-        <v>0.175</v>
+        <v>0.102</v>
       </c>
       <c r="D77">
-        <v>0.603</v>
+        <v>1.034</v>
       </c>
       <c r="E77">
-        <v>0.5479999999999999</v>
+        <v>0.301</v>
       </c>
       <c r="F77">
-        <v>-0.242</v>
+        <v>-0.095</v>
       </c>
       <c r="G77">
-        <v>0.453</v>
+        <v>0.306</v>
       </c>
       <c r="H77" t="s">
         <v>25</v>
@@ -2477,16 +2477,16 @@
         <v>-0.0202</v>
       </c>
       <c r="C78">
-        <v>0.019</v>
+        <v>0.02</v>
       </c>
       <c r="D78">
-        <v>-1.056</v>
+        <v>-1.025</v>
       </c>
       <c r="E78">
-        <v>0.293</v>
+        <v>0.305</v>
       </c>
       <c r="F78">
-        <v>-0.058</v>
+        <v>-0.059</v>
       </c>
       <c r="G78">
         <v>0.018</v>
@@ -2503,19 +2503,19 @@
         <v>0.0159</v>
       </c>
       <c r="C79">
-        <v>0.031</v>
+        <v>0.013</v>
       </c>
       <c r="D79">
-        <v>0.512</v>
+        <v>1.203</v>
       </c>
       <c r="E79">
-        <v>0.61</v>
+        <v>0.229</v>
       </c>
       <c r="F79">
-        <v>-0.046</v>
+        <v>-0.01</v>
       </c>
       <c r="G79">
-        <v>0.078</v>
+        <v>0.042</v>
       </c>
       <c r="H79" t="s">
         <v>25</v>
@@ -2529,19 +2529,19 @@
         <v>0.1735</v>
       </c>
       <c r="C80">
-        <v>0.391</v>
+        <v>0.399</v>
       </c>
       <c r="D80">
-        <v>0.444</v>
+        <v>0.435</v>
       </c>
       <c r="E80">
-        <v>0.6579999999999999</v>
+        <v>0.664</v>
       </c>
       <c r="F80">
-        <v>-0.602</v>
+        <v>-0.608</v>
       </c>
       <c r="G80">
-        <v>0.9490000000000001</v>
+        <v>0.955</v>
       </c>
       <c r="H80" t="s">
         <v>26</v>
@@ -2558,16 +2558,16 @@
         <v>0.034</v>
       </c>
       <c r="D81">
-        <v>-0.303</v>
+        <v>-0.305</v>
       </c>
       <c r="E81">
-        <v>0.762</v>
+        <v>0.76</v>
       </c>
       <c r="F81">
-        <v>-0.079</v>
+        <v>-0.078</v>
       </c>
       <c r="G81">
-        <v>0.058</v>
+        <v>0.057</v>
       </c>
       <c r="H81" t="s">
         <v>26</v>
@@ -2581,19 +2581,19 @@
         <v>-0.0008</v>
       </c>
       <c r="C82">
-        <v>0.065</v>
+        <v>0.067</v>
       </c>
       <c r="D82">
-        <v>-0.012</v>
+        <v>-0.011</v>
       </c>
       <c r="E82">
         <v>0.991</v>
       </c>
       <c r="F82">
-        <v>-0.129</v>
+        <v>-0.132</v>
       </c>
       <c r="G82">
-        <v>0.128</v>
+        <v>0.13</v>
       </c>
       <c r="H82" t="s">
         <v>26</v>
@@ -2610,10 +2610,10 @@
         <v>0.004</v>
       </c>
       <c r="D83">
-        <v>1.694</v>
+        <v>1.807</v>
       </c>
       <c r="E83">
-        <v>0.09300000000000001</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="F83">
         <v>-0.001</v>
@@ -2633,19 +2633,19 @@
         <v>0.008</v>
       </c>
       <c r="C84">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
       <c r="D84">
-        <v>0.524</v>
+        <v>0.44</v>
       </c>
       <c r="E84">
-        <v>0.602</v>
+        <v>0.66</v>
       </c>
       <c r="F84">
-        <v>-0.022</v>
+        <v>-0.028</v>
       </c>
       <c r="G84">
-        <v>0.038</v>
+        <v>0.044</v>
       </c>
       <c r="H84" t="s">
         <v>26</v>
@@ -2659,19 +2659,19 @@
         <v>-0.0027</v>
       </c>
       <c r="C85">
-        <v>0.006999999999999999</v>
+        <v>0.004</v>
       </c>
       <c r="D85">
-        <v>-0.391</v>
+        <v>-0.705</v>
       </c>
       <c r="E85">
-        <v>0.6970000000000001</v>
+        <v>0.481</v>
       </c>
       <c r="F85">
-        <v>-0.016</v>
+        <v>-0.01</v>
       </c>
       <c r="G85">
-        <v>0.011</v>
+        <v>0.005</v>
       </c>
       <c r="H85" t="s">
         <v>26</v>
@@ -2685,19 +2685,19 @@
         <v>-0.005</v>
       </c>
       <c r="C86">
-        <v>0.014</v>
+        <v>0.016</v>
       </c>
       <c r="D86">
-        <v>-0.355</v>
+        <v>-0.315</v>
       </c>
       <c r="E86">
-        <v>0.723</v>
+        <v>0.753</v>
       </c>
       <c r="F86">
-        <v>-0.033</v>
+        <v>-0.036</v>
       </c>
       <c r="G86">
-        <v>0.023</v>
+        <v>0.026</v>
       </c>
       <c r="H86" t="s">
         <v>26</v>
@@ -2711,19 +2711,19 @@
         <v>0.0002</v>
       </c>
       <c r="C87">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
       <c r="D87">
-        <v>0.029</v>
+        <v>0.038</v>
       </c>
       <c r="E87">
-        <v>0.977</v>
+        <v>0.97</v>
       </c>
       <c r="F87">
-        <v>-0.016</v>
+        <v>-0.012</v>
       </c>
       <c r="G87">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="H87" t="s">
         <v>26</v>
@@ -2740,16 +2740,16 @@
         <v>0.004</v>
       </c>
       <c r="D88">
-        <v>0.09</v>
+        <v>0.103</v>
       </c>
       <c r="E88">
-        <v>0.9279999999999999</v>
+        <v>0.9179999999999999</v>
       </c>
       <c r="F88">
-        <v>-0.008</v>
+        <v>-0.006999999999999999</v>
       </c>
       <c r="G88">
-        <v>0.009000000000000001</v>
+        <v>0.008</v>
       </c>
       <c r="H88" t="s">
         <v>26</v>
@@ -2763,19 +2763,19 @@
         <v>0.0043</v>
       </c>
       <c r="C89">
-        <v>0.03700000000000001</v>
+        <v>0.046</v>
       </c>
       <c r="D89">
-        <v>0.116</v>
+        <v>0.092</v>
       </c>
       <c r="E89">
-        <v>0.9079999999999999</v>
+        <v>0.927</v>
       </c>
       <c r="F89">
-        <v>-0.06900000000000001</v>
+        <v>-0.08699999999999999</v>
       </c>
       <c r="G89">
-        <v>0.077</v>
+        <v>0.095</v>
       </c>
       <c r="H89" t="s">
         <v>26</v>
@@ -2789,19 +2789,19 @@
         <v>0.0465</v>
       </c>
       <c r="C90">
-        <v>0.048</v>
+        <v>0.043</v>
       </c>
       <c r="D90">
-        <v>0.976</v>
+        <v>1.071</v>
       </c>
       <c r="E90">
-        <v>0.331</v>
+        <v>0.284</v>
       </c>
       <c r="F90">
-        <v>-0.048</v>
+        <v>-0.039</v>
       </c>
       <c r="G90">
-        <v>0.141</v>
+        <v>0.132</v>
       </c>
       <c r="H90" t="s">
         <v>26</v>
@@ -2815,19 +2815,19 @@
         <v>-0.008200000000000001</v>
       </c>
       <c r="C91">
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
       <c r="D91">
-        <v>-1.571</v>
+        <v>-1.444</v>
       </c>
       <c r="E91">
-        <v>0.119</v>
+        <v>0.149</v>
       </c>
       <c r="F91">
         <v>-0.019</v>
       </c>
       <c r="G91">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="H91" t="s">
         <v>26</v>
@@ -2844,10 +2844,10 @@
         <v>0.008</v>
       </c>
       <c r="D92">
-        <v>0.206</v>
+        <v>0.209</v>
       </c>
       <c r="E92">
-        <v>0.8370000000000001</v>
+        <v>0.8340000000000001</v>
       </c>
       <c r="F92">
         <v>-0.015</v>
@@ -2867,19 +2867,19 @@
         <v>0.5477</v>
       </c>
       <c r="C93">
-        <v>0.333</v>
+        <v>0.256</v>
       </c>
       <c r="D93">
-        <v>1.647</v>
+        <v>2.141</v>
       </c>
       <c r="E93">
-        <v>0.103</v>
+        <v>0.032</v>
       </c>
       <c r="F93">
-        <v>-0.112</v>
+        <v>0.046</v>
       </c>
       <c r="G93">
-        <v>1.207</v>
+        <v>1.049</v>
       </c>
       <c r="H93" t="s">
         <v>27</v>
@@ -2893,19 +2893,19 @@
         <v>0.0042</v>
       </c>
       <c r="C94">
-        <v>0.029</v>
+        <v>0.023</v>
       </c>
       <c r="D94">
-        <v>0.142</v>
+        <v>0.18</v>
       </c>
       <c r="E94">
-        <v>0.887</v>
+        <v>0.857</v>
       </c>
       <c r="F94">
-        <v>-0.05400000000000001</v>
+        <v>-0.04099999999999999</v>
       </c>
       <c r="G94">
-        <v>0.062</v>
+        <v>0.049</v>
       </c>
       <c r="H94" t="s">
         <v>27</v>
@@ -2919,19 +2919,19 @@
         <v>-0.0169</v>
       </c>
       <c r="C95">
-        <v>0.055</v>
+        <v>0.038</v>
       </c>
       <c r="D95">
-        <v>-0.307</v>
+        <v>-0.451</v>
       </c>
       <c r="E95">
-        <v>0.759</v>
+        <v>0.652</v>
       </c>
       <c r="F95">
-        <v>-0.126</v>
+        <v>-0.09</v>
       </c>
       <c r="G95">
-        <v>0.092</v>
+        <v>0.057</v>
       </c>
       <c r="H95" t="s">
         <v>27</v>
@@ -2945,19 +2945,19 @@
         <v>-0.001</v>
       </c>
       <c r="C96">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="D96">
-        <v>-0.304</v>
+        <v>-0.409</v>
       </c>
       <c r="E96">
-        <v>0.762</v>
+        <v>0.6829999999999999</v>
       </c>
       <c r="F96">
-        <v>-0.008</v>
+        <v>-0.006</v>
       </c>
       <c r="G96">
-        <v>0.006</v>
+        <v>0.004</v>
       </c>
       <c r="H96" t="s">
         <v>27</v>
@@ -2971,19 +2971,19 @@
         <v>-0.0132</v>
       </c>
       <c r="C97">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
       <c r="D97">
-        <v>-1.022</v>
+        <v>-0.956</v>
       </c>
       <c r="E97">
-        <v>0.309</v>
+        <v>0.339</v>
       </c>
       <c r="F97">
-        <v>-0.039</v>
+        <v>-0.04</v>
       </c>
       <c r="G97">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
       <c r="H97" t="s">
         <v>27</v>
@@ -2997,19 +2997,19 @@
         <v>-0.0059</v>
       </c>
       <c r="C98">
-        <v>0.006</v>
+        <v>0.003</v>
       </c>
       <c r="D98">
-        <v>-0.997</v>
+        <v>-2.311</v>
       </c>
       <c r="E98">
-        <v>0.321</v>
+        <v>0.021</v>
       </c>
       <c r="F98">
-        <v>-0.018</v>
+        <v>-0.011</v>
       </c>
       <c r="G98">
-        <v>0.006</v>
+        <v>-0.001</v>
       </c>
       <c r="H98" t="s">
         <v>27</v>
@@ -3023,19 +3023,19 @@
         <v>-0.0202</v>
       </c>
       <c r="C99">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="D99">
-        <v>-1.674</v>
+        <v>-1.873</v>
       </c>
       <c r="E99">
-        <v>0.09699999999999999</v>
+        <v>0.061</v>
       </c>
       <c r="F99">
-        <v>-0.044</v>
+        <v>-0.04099999999999999</v>
       </c>
       <c r="G99">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="H99" t="s">
         <v>27</v>
@@ -3049,19 +3049,19 @@
         <v>0.009900000000000001</v>
       </c>
       <c r="C100">
-        <v>0.006999999999999999</v>
+        <v>0.006</v>
       </c>
       <c r="D100">
-        <v>1.427</v>
+        <v>1.785</v>
       </c>
       <c r="E100">
-        <v>0.156</v>
+        <v>0.07400000000000001</v>
       </c>
       <c r="F100">
-        <v>-0.004</v>
+        <v>-0.001</v>
       </c>
       <c r="G100">
-        <v>0.024</v>
+        <v>0.021</v>
       </c>
       <c r="H100" t="s">
         <v>27</v>
@@ -3075,19 +3075,19 @@
         <v>-0.008399999999999999</v>
       </c>
       <c r="C101">
+        <v>0.003</v>
+      </c>
+      <c r="D101">
+        <v>-2.88</v>
+      </c>
+      <c r="E101">
         <v>0.004</v>
       </c>
-      <c r="D101">
-        <v>-2.27</v>
-      </c>
-      <c r="E101">
-        <v>0.025</v>
-      </c>
       <c r="F101">
-        <v>-0.016</v>
+        <v>-0.014</v>
       </c>
       <c r="G101">
-        <v>-0.001</v>
+        <v>-0.003</v>
       </c>
       <c r="H101" t="s">
         <v>27</v>
@@ -3101,19 +3101,19 @@
         <v>-0.0067</v>
       </c>
       <c r="C102">
-        <v>0.031</v>
+        <v>0.033</v>
       </c>
       <c r="D102">
-        <v>-0.215</v>
+        <v>-0.201</v>
       </c>
       <c r="E102">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="F102">
-        <v>-0.06900000000000001</v>
+        <v>-0.07200000000000001</v>
       </c>
       <c r="G102">
-        <v>0.055</v>
+        <v>0.059</v>
       </c>
       <c r="H102" t="s">
         <v>27</v>
@@ -3127,19 +3127,19 @@
         <v>0.0558</v>
       </c>
       <c r="C103">
-        <v>0.04099999999999999</v>
+        <v>0.031</v>
       </c>
       <c r="D103">
-        <v>1.375</v>
+        <v>1.776</v>
       </c>
       <c r="E103">
-        <v>0.172</v>
+        <v>0.076</v>
       </c>
       <c r="F103">
-        <v>-0.025</v>
+        <v>-0.006</v>
       </c>
       <c r="G103">
-        <v>0.136</v>
+        <v>0.117</v>
       </c>
       <c r="H103" t="s">
         <v>27</v>
@@ -3156,16 +3156,16 @@
         <v>0.004</v>
       </c>
       <c r="D104">
-        <v>-0.237</v>
+        <v>-0.279</v>
       </c>
       <c r="E104">
-        <v>0.8129999999999999</v>
+        <v>0.78</v>
       </c>
       <c r="F104">
-        <v>-0.01</v>
+        <v>-0.008</v>
       </c>
       <c r="G104">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
       <c r="H104" t="s">
         <v>27</v>
@@ -3179,19 +3179,19 @@
         <v>-0.008699999999999999</v>
       </c>
       <c r="C105">
-        <v>0.006999999999999999</v>
+        <v>0.005</v>
       </c>
       <c r="D105">
-        <v>-1.209</v>
+        <v>-1.837</v>
       </c>
       <c r="E105">
-        <v>0.23</v>
+        <v>0.066</v>
       </c>
       <c r="F105">
-        <v>-0.023</v>
+        <v>-0.018</v>
       </c>
       <c r="G105">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
       <c r="H105" t="s">
         <v>27</v>
@@ -3205,19 +3205,19 @@
         <v>-2.4659</v>
       </c>
       <c r="C106">
-        <v>1.394</v>
+        <v>2.423</v>
       </c>
       <c r="D106">
-        <v>-1.769</v>
+        <v>-1.018</v>
       </c>
       <c r="E106">
-        <v>0.08</v>
+        <v>0.309</v>
       </c>
       <c r="F106">
-        <v>-5.23</v>
+        <v>-7.215</v>
       </c>
       <c r="G106">
-        <v>0.298</v>
+        <v>2.283</v>
       </c>
       <c r="H106" t="s">
         <v>28</v>
@@ -3231,19 +3231,19 @@
         <v>-0.0115</v>
       </c>
       <c r="C107">
-        <v>0.123</v>
+        <v>0.094</v>
       </c>
       <c r="D107">
-        <v>-0.094</v>
+        <v>-0.122</v>
       </c>
       <c r="E107">
-        <v>0.9259999999999999</v>
+        <v>0.903</v>
       </c>
       <c r="F107">
-        <v>-0.255</v>
+        <v>-0.196</v>
       </c>
       <c r="G107">
-        <v>0.232</v>
+        <v>0.173</v>
       </c>
       <c r="H107" t="s">
         <v>28</v>
@@ -3257,19 +3257,19 @@
         <v>-0.2515</v>
       </c>
       <c r="C108">
-        <v>0.231</v>
+        <v>0.194</v>
       </c>
       <c r="D108">
-        <v>-1.088</v>
+        <v>-1.294</v>
       </c>
       <c r="E108">
-        <v>0.279</v>
+        <v>0.196</v>
       </c>
       <c r="F108">
-        <v>-0.71</v>
+        <v>-0.632</v>
       </c>
       <c r="G108">
-        <v>0.207</v>
+        <v>0.129</v>
       </c>
       <c r="H108" t="s">
         <v>28</v>
@@ -3283,19 +3283,19 @@
         <v>0.0029</v>
       </c>
       <c r="C109">
-        <v>0.014</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="D109">
-        <v>0.209</v>
+        <v>0.405</v>
       </c>
       <c r="E109">
-        <v>0.835</v>
+        <v>0.6859999999999999</v>
       </c>
       <c r="F109">
-        <v>-0.024</v>
+        <v>-0.011</v>
       </c>
       <c r="G109">
-        <v>0.03</v>
+        <v>0.017</v>
       </c>
       <c r="H109" t="s">
         <v>28</v>
@@ -3309,19 +3309,19 @@
         <v>0.109</v>
       </c>
       <c r="C110">
-        <v>0.05400000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="D110">
-        <v>2.009</v>
+        <v>0.9890000000000001</v>
       </c>
       <c r="E110">
-        <v>0.047</v>
+        <v>0.323</v>
       </c>
       <c r="F110">
-        <v>0.001</v>
+        <v>-0.107</v>
       </c>
       <c r="G110">
-        <v>0.217</v>
+        <v>0.325</v>
       </c>
       <c r="H110" t="s">
         <v>28</v>
@@ -3335,19 +3335,19 @@
         <v>0.001</v>
       </c>
       <c r="C111">
-        <v>0.025</v>
+        <v>0.02</v>
       </c>
       <c r="D111">
-        <v>0.042</v>
+        <v>0.053</v>
       </c>
       <c r="E111">
-        <v>0.9670000000000001</v>
+        <v>0.958</v>
       </c>
       <c r="F111">
-        <v>-0.048</v>
+        <v>-0.03700000000000001</v>
       </c>
       <c r="G111">
-        <v>0.05</v>
+        <v>0.039</v>
       </c>
       <c r="H111" t="s">
         <v>28</v>
@@ -3361,19 +3361,19 @@
         <v>0.0849</v>
       </c>
       <c r="C112">
-        <v>0.051</v>
+        <v>0.079</v>
       </c>
       <c r="D112">
-        <v>1.675</v>
+        <v>1.078</v>
       </c>
       <c r="E112">
-        <v>0.09699999999999999</v>
+        <v>0.281</v>
       </c>
       <c r="F112">
-        <v>-0.016</v>
+        <v>-0.06900000000000001</v>
       </c>
       <c r="G112">
-        <v>0.185</v>
+        <v>0.239</v>
       </c>
       <c r="H112" t="s">
         <v>28</v>
@@ -3387,19 +3387,19 @@
         <v>-0.0095</v>
       </c>
       <c r="C113">
-        <v>0.029</v>
+        <v>0.018</v>
       </c>
       <c r="D113">
-        <v>-0.324</v>
+        <v>-0.536</v>
       </c>
       <c r="E113">
-        <v>0.747</v>
+        <v>0.5920000000000001</v>
       </c>
       <c r="F113">
-        <v>-0.067</v>
+        <v>-0.044</v>
       </c>
       <c r="G113">
-        <v>0.048</v>
+        <v>0.025</v>
       </c>
       <c r="H113" t="s">
         <v>28</v>
@@ -3413,19 +3413,19 @@
         <v>0.0111</v>
       </c>
       <c r="C114">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="D114">
-        <v>0.7140000000000001</v>
+        <v>0.795</v>
       </c>
       <c r="E114">
-        <v>0.477</v>
+        <v>0.427</v>
       </c>
       <c r="F114">
-        <v>-0.02</v>
+        <v>-0.016</v>
       </c>
       <c r="G114">
-        <v>0.042</v>
+        <v>0.038</v>
       </c>
       <c r="H114" t="s">
         <v>28</v>
@@ -3439,19 +3439,19 @@
         <v>0.3999</v>
       </c>
       <c r="C115">
-        <v>0.131</v>
+        <v>0.278</v>
       </c>
       <c r="D115">
-        <v>3.054</v>
+        <v>1.438</v>
       </c>
       <c r="E115">
-        <v>0.003</v>
+        <v>0.151</v>
       </c>
       <c r="F115">
-        <v>0.14</v>
+        <v>-0.145</v>
       </c>
       <c r="G115">
-        <v>0.66</v>
+        <v>0.945</v>
       </c>
       <c r="H115" t="s">
         <v>28</v>
@@ -3465,19 +3465,19 @@
         <v>-0.0095</v>
       </c>
       <c r="C116">
-        <v>0.17</v>
+        <v>0.081</v>
       </c>
       <c r="D116">
-        <v>-0.05599999999999999</v>
+        <v>-0.118</v>
       </c>
       <c r="E116">
-        <v>0.955</v>
+        <v>0.9059999999999999</v>
       </c>
       <c r="F116">
-        <v>-0.346</v>
+        <v>-0.168</v>
       </c>
       <c r="G116">
-        <v>0.327</v>
+        <v>0.149</v>
       </c>
       <c r="H116" t="s">
         <v>28</v>
@@ -3494,16 +3494,16 @@
         <v>0.019</v>
       </c>
       <c r="D117">
-        <v>0.625</v>
+        <v>0.616</v>
       </c>
       <c r="E117">
-        <v>0.534</v>
+        <v>0.5379999999999999</v>
       </c>
       <c r="F117">
         <v>-0.025</v>
       </c>
       <c r="G117">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="H117" t="s">
         <v>28</v>
@@ -3517,19 +3517,19 @@
         <v>0.0003</v>
       </c>
       <c r="C118">
-        <v>0.03</v>
+        <v>0.013</v>
       </c>
       <c r="D118">
-        <v>0.009000000000000001</v>
+        <v>0.021</v>
       </c>
       <c r="E118">
-        <v>0.993</v>
+        <v>0.983</v>
       </c>
       <c r="F118">
-        <v>-0.059</v>
+        <v>-0.025</v>
       </c>
       <c r="G118">
-        <v>0.06</v>
+        <v>0.025</v>
       </c>
       <c r="H118" t="s">
         <v>28</v>
@@ -3543,19 +3543,19 @@
         <v>2.9524</v>
       </c>
       <c r="C119">
-        <v>1.329</v>
+        <v>2.217</v>
       </c>
       <c r="D119">
-        <v>2.222</v>
+        <v>1.332</v>
       </c>
       <c r="E119">
-        <v>0.028</v>
+        <v>0.183</v>
       </c>
       <c r="F119">
-        <v>0.319</v>
+        <v>-1.393</v>
       </c>
       <c r="G119">
-        <v>5.586</v>
+        <v>7.297000000000001</v>
       </c>
       <c r="H119" t="s">
         <v>29</v>
@@ -3569,19 +3569,19 @@
         <v>0.0709</v>
       </c>
       <c r="C120">
-        <v>0.117</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="D120">
-        <v>0.606</v>
+        <v>0.838</v>
       </c>
       <c r="E120">
-        <v>0.546</v>
+        <v>0.402</v>
       </c>
       <c r="F120">
-        <v>-0.161</v>
+        <v>-0.095</v>
       </c>
       <c r="G120">
-        <v>0.303</v>
+        <v>0.237</v>
       </c>
       <c r="H120" t="s">
         <v>29</v>
@@ -3595,19 +3595,19 @@
         <v>0.1121</v>
       </c>
       <c r="C121">
-        <v>0.22</v>
+        <v>0.174</v>
       </c>
       <c r="D121">
-        <v>0.509</v>
+        <v>0.645</v>
       </c>
       <c r="E121">
-        <v>0.612</v>
+        <v>0.519</v>
       </c>
       <c r="F121">
-        <v>-0.324</v>
+        <v>-0.228</v>
       </c>
       <c r="G121">
-        <v>0.5489999999999999</v>
+        <v>0.453</v>
       </c>
       <c r="H121" t="s">
         <v>29</v>
@@ -3621,19 +3621,19 @@
         <v>0.0007</v>
       </c>
       <c r="C122">
+        <v>0.006</v>
+      </c>
+      <c r="D122">
+        <v>0.103</v>
+      </c>
+      <c r="E122">
+        <v>0.9179999999999999</v>
+      </c>
+      <c r="F122">
+        <v>-0.012</v>
+      </c>
+      <c r="G122">
         <v>0.013</v>
-      </c>
-      <c r="D122">
-        <v>0.05</v>
-      </c>
-      <c r="E122">
-        <v>0.96</v>
-      </c>
-      <c r="F122">
-        <v>-0.025</v>
-      </c>
-      <c r="G122">
-        <v>0.027</v>
       </c>
       <c r="H122" t="s">
         <v>29</v>
@@ -3647,19 +3647,19 @@
         <v>-0.142</v>
       </c>
       <c r="C123">
-        <v>0.052</v>
+        <v>0.104</v>
       </c>
       <c r="D123">
-        <v>-2.745</v>
+        <v>-1.36</v>
       </c>
       <c r="E123">
-        <v>0.006999999999999999</v>
+        <v>0.174</v>
       </c>
       <c r="F123">
-        <v>-0.245</v>
+        <v>-0.347</v>
       </c>
       <c r="G123">
-        <v>-0.039</v>
+        <v>0.063</v>
       </c>
       <c r="H123" t="s">
         <v>29</v>
@@ -3673,19 +3673,19 @@
         <v>-0.0008</v>
       </c>
       <c r="C124">
-        <v>0.024</v>
+        <v>0.014</v>
       </c>
       <c r="D124">
-        <v>-0.035</v>
+        <v>-0.058</v>
       </c>
       <c r="E124">
-        <v>0.972</v>
+        <v>0.9540000000000001</v>
       </c>
       <c r="F124">
-        <v>-0.048</v>
+        <v>-0.029</v>
       </c>
       <c r="G124">
-        <v>0.046</v>
+        <v>0.027</v>
       </c>
       <c r="H124" t="s">
         <v>29</v>
@@ -3699,19 +3699,19 @@
         <v>-0.1062</v>
       </c>
       <c r="C125">
-        <v>0.048</v>
+        <v>0.07400000000000001</v>
       </c>
       <c r="D125">
-        <v>-2.199</v>
+        <v>-1.442</v>
       </c>
       <c r="E125">
-        <v>0.03</v>
+        <v>0.149</v>
       </c>
       <c r="F125">
-        <v>-0.202</v>
+        <v>-0.251</v>
       </c>
       <c r="G125">
-        <v>-0.01</v>
+        <v>0.038</v>
       </c>
       <c r="H125" t="s">
         <v>29</v>
@@ -3725,19 +3725,19 @@
         <v>0.0025</v>
       </c>
       <c r="C126">
-        <v>0.028</v>
+        <v>0.018</v>
       </c>
       <c r="D126">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
       <c r="E126">
-        <v>0.9279999999999999</v>
+        <v>0.888</v>
       </c>
       <c r="F126">
-        <v>-0.053</v>
+        <v>-0.033</v>
       </c>
       <c r="G126">
-        <v>0.058</v>
+        <v>0.038</v>
       </c>
       <c r="H126" t="s">
         <v>29</v>
@@ -3751,19 +3751,19 @@
         <v>-0.0122</v>
       </c>
       <c r="C127">
-        <v>0.015</v>
+        <v>0.013</v>
       </c>
       <c r="D127">
-        <v>-0.8290000000000001</v>
+        <v>-0.955</v>
       </c>
       <c r="E127">
-        <v>0.409</v>
+        <v>0.339</v>
       </c>
       <c r="F127">
-        <v>-0.04099999999999999</v>
+        <v>-0.03700000000000001</v>
       </c>
       <c r="G127">
-        <v>0.017</v>
+        <v>0.013</v>
       </c>
       <c r="H127" t="s">
         <v>29</v>
@@ -3777,19 +3777,19 @@
         <v>-0.29</v>
       </c>
       <c r="C128">
-        <v>0.125</v>
+        <v>0.26</v>
       </c>
       <c r="D128">
-        <v>-2.324</v>
+        <v>-1.117</v>
       </c>
       <c r="E128">
-        <v>0.022</v>
+        <v>0.264</v>
       </c>
       <c r="F128">
-        <v>-0.537</v>
+        <v>-0.799</v>
       </c>
       <c r="G128">
-        <v>-0.043</v>
+        <v>0.219</v>
       </c>
       <c r="H128" t="s">
         <v>29</v>
@@ -3803,19 +3803,19 @@
         <v>0.1242</v>
       </c>
       <c r="C129">
-        <v>0.162</v>
+        <v>0.076</v>
       </c>
       <c r="D129">
-        <v>0.767</v>
+        <v>1.644</v>
       </c>
       <c r="E129">
-        <v>0.445</v>
+        <v>0.1</v>
       </c>
       <c r="F129">
-        <v>-0.197</v>
+        <v>-0.024</v>
       </c>
       <c r="G129">
-        <v>0.445</v>
+        <v>0.272</v>
       </c>
       <c r="H129" t="s">
         <v>29</v>
@@ -3835,10 +3835,10 @@
         <v>-1.504</v>
       </c>
       <c r="E130">
-        <v>0.135</v>
+        <v>0.132</v>
       </c>
       <c r="F130">
-        <v>-0.062</v>
+        <v>-0.061</v>
       </c>
       <c r="G130">
         <v>0.008</v>
@@ -3855,19 +3855,19 @@
         <v>0.0197</v>
       </c>
       <c r="C131">
-        <v>0.029</v>
+        <v>0.014</v>
       </c>
       <c r="D131">
-        <v>0.6859999999999999</v>
+        <v>1.441</v>
       </c>
       <c r="E131">
-        <v>0.494</v>
+        <v>0.15</v>
       </c>
       <c r="F131">
-        <v>-0.03700000000000001</v>
+        <v>-0.006999999999999999</v>
       </c>
       <c r="G131">
-        <v>0.077</v>
+        <v>0.047</v>
       </c>
       <c r="H131" t="s">
         <v>29</v>
@@ -3881,19 +3881,19 @@
         <v>0.6368</v>
       </c>
       <c r="C132">
-        <v>0.46</v>
+        <v>0.606</v>
       </c>
       <c r="D132">
-        <v>1.384</v>
+        <v>1.051</v>
       </c>
       <c r="E132">
-        <v>0.169</v>
+        <v>0.293</v>
       </c>
       <c r="F132">
-        <v>-0.275</v>
+        <v>-0.551</v>
       </c>
       <c r="G132">
-        <v>1.549</v>
+        <v>1.824</v>
       </c>
       <c r="H132" t="s">
         <v>30</v>
@@ -3907,19 +3907,19 @@
         <v>-0.0418</v>
       </c>
       <c r="C133">
-        <v>0.04099999999999999</v>
+        <v>0.03</v>
       </c>
       <c r="D133">
-        <v>-1.031</v>
+        <v>-1.416</v>
       </c>
       <c r="E133">
-        <v>0.305</v>
+        <v>0.157</v>
       </c>
       <c r="F133">
-        <v>-0.122</v>
+        <v>-0.1</v>
       </c>
       <c r="G133">
-        <v>0.039</v>
+        <v>0.016</v>
       </c>
       <c r="H133" t="s">
         <v>30</v>
@@ -3933,19 +3933,19 @@
         <v>-0.0106</v>
       </c>
       <c r="C134">
-        <v>0.076</v>
+        <v>0.062</v>
       </c>
       <c r="D134">
-        <v>-0.139</v>
+        <v>-0.17</v>
       </c>
       <c r="E134">
-        <v>0.89</v>
+        <v>0.865</v>
       </c>
       <c r="F134">
-        <v>-0.162</v>
+        <v>-0.133</v>
       </c>
       <c r="G134">
-        <v>0.141</v>
+        <v>0.111</v>
       </c>
       <c r="H134" t="s">
         <v>30</v>
@@ -3959,19 +3959,19 @@
         <v>0.0034</v>
       </c>
       <c r="C135">
-        <v>0.005</v>
+        <v>0.003</v>
       </c>
       <c r="D135">
-        <v>0.743</v>
+        <v>1.304</v>
       </c>
       <c r="E135">
-        <v>0.459</v>
+        <v>0.192</v>
       </c>
       <c r="F135">
-        <v>-0.006</v>
+        <v>-0.002</v>
       </c>
       <c r="G135">
-        <v>0.012</v>
+        <v>0.008</v>
       </c>
       <c r="H135" t="s">
         <v>30</v>
@@ -3985,19 +3985,19 @@
         <v>-0.041</v>
       </c>
       <c r="C136">
-        <v>0.018</v>
+        <v>0.029</v>
       </c>
       <c r="D136">
-        <v>-2.287</v>
+        <v>-1.391</v>
       </c>
       <c r="E136">
-        <v>0.024</v>
+        <v>0.164</v>
       </c>
       <c r="F136">
-        <v>-0.076</v>
+        <v>-0.099</v>
       </c>
       <c r="G136">
-        <v>-0.005</v>
+        <v>0.017</v>
       </c>
       <c r="H136" t="s">
         <v>30</v>
@@ -4011,19 +4011,19 @@
         <v>0.0032</v>
       </c>
       <c r="C137">
-        <v>0.008</v>
+        <v>0.003</v>
       </c>
       <c r="D137">
-        <v>0.386</v>
+        <v>0.975</v>
       </c>
       <c r="E137">
-        <v>0.7</v>
+        <v>0.33</v>
       </c>
       <c r="F137">
-        <v>-0.013</v>
+        <v>-0.003</v>
       </c>
       <c r="G137">
-        <v>0.019</v>
+        <v>0.009000000000000001</v>
       </c>
       <c r="H137" t="s">
         <v>30</v>
@@ -4037,19 +4037,19 @@
         <v>-0.022</v>
       </c>
       <c r="C138">
-        <v>0.017</v>
+        <v>0.022</v>
       </c>
       <c r="D138">
-        <v>-1.316</v>
+        <v>-1.014</v>
       </c>
       <c r="E138">
-        <v>0.191</v>
+        <v>0.31</v>
       </c>
       <c r="F138">
-        <v>-0.055</v>
+        <v>-0.065</v>
       </c>
       <c r="G138">
-        <v>0.011</v>
+        <v>0.021</v>
       </c>
       <c r="H138" t="s">
         <v>30</v>
@@ -4063,19 +4063,19 @@
         <v>0.0039</v>
       </c>
       <c r="C139">
-        <v>0.01</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="D139">
-        <v>0.403</v>
+        <v>0.5589999999999999</v>
       </c>
       <c r="E139">
-        <v>0.6879999999999999</v>
+        <v>0.5760000000000001</v>
       </c>
       <c r="F139">
-        <v>-0.015</v>
+        <v>-0.01</v>
       </c>
       <c r="G139">
-        <v>0.023</v>
+        <v>0.017</v>
       </c>
       <c r="H139" t="s">
         <v>30</v>
@@ -4092,16 +4092,16 @@
         <v>0.005</v>
       </c>
       <c r="D140">
-        <v>-1.607</v>
+        <v>-1.79</v>
       </c>
       <c r="E140">
-        <v>0.111</v>
+        <v>0.073</v>
       </c>
       <c r="F140">
-        <v>-0.018</v>
+        <v>-0.017</v>
       </c>
       <c r="G140">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="H140" t="s">
         <v>30</v>
@@ -4115,19 +4115,19 @@
         <v>-0.0945</v>
       </c>
       <c r="C141">
-        <v>0.043</v>
+        <v>0.07400000000000001</v>
       </c>
       <c r="D141">
-        <v>-2.187</v>
+        <v>-1.285</v>
       </c>
       <c r="E141">
-        <v>0.031</v>
+        <v>0.199</v>
       </c>
       <c r="F141">
-        <v>-0.18</v>
+        <v>-0.239</v>
       </c>
       <c r="G141">
-        <v>-0.009000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="H141" t="s">
         <v>30</v>
@@ -4141,19 +4141,19 @@
         <v>0.0324</v>
       </c>
       <c r="C142">
-        <v>0.05599999999999999</v>
+        <v>0.034</v>
       </c>
       <c r="D142">
-        <v>0.578</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E142">
-        <v>0.5649999999999999</v>
+        <v>0.347</v>
       </c>
       <c r="F142">
-        <v>-0.079</v>
+        <v>-0.035</v>
       </c>
       <c r="G142">
-        <v>0.144</v>
+        <v>0.1</v>
       </c>
       <c r="H142" t="s">
         <v>30</v>
@@ -4167,19 +4167,19 @@
         <v>-0.0062</v>
       </c>
       <c r="C143">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="D143">
-        <v>-1.016</v>
+        <v>-1.149</v>
       </c>
       <c r="E143">
-        <v>0.312</v>
+        <v>0.251</v>
       </c>
       <c r="F143">
-        <v>-0.018</v>
+        <v>-0.017</v>
       </c>
       <c r="G143">
-        <v>0.006</v>
+        <v>0.004</v>
       </c>
       <c r="H143" t="s">
         <v>30</v>
@@ -4193,19 +4193,19 @@
         <v>-0.0008</v>
       </c>
       <c r="C144">
-        <v>0.01</v>
+        <v>0.006</v>
       </c>
       <c r="D144">
-        <v>-0.08199999999999999</v>
+        <v>-0.131</v>
       </c>
       <c r="E144">
-        <v>0.9350000000000001</v>
+        <v>0.8959999999999999</v>
       </c>
       <c r="F144">
-        <v>-0.021</v>
+        <v>-0.013</v>
       </c>
       <c r="G144">
-        <v>0.019</v>
+        <v>0.011</v>
       </c>
       <c r="H144" t="s">
         <v>30</v>

</xml_diff>